<commit_message>
Added joined DF for models
</commit_message>
<xml_diff>
--- a/data/raw/band_populations.xlsx
+++ b/data/raw/band_populations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/_waapihk/nan_remoteness/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://validuseconomicscom.sharepoint.com/sites/WaapihkResearch/Shared Documents/General/Client &amp; Project Folders/AMC/Education/REA/Enhancements/Remoteness/Nishnawbe Aski Nation Remoteness Approach for AMC/sources/R/nan_remoteness/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1AC2F9-0CB4-D643-9679-25F66E516723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{8A1AC2F9-0CB4-D643-9679-25F66E516723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FEE4534-0C75-7849-B28D-97A7888E7378}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{686AE0AF-66C7-0740-AB43-CE4D07826517}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>First Nation</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Source URL</t>
+  </si>
+  <si>
+    <t>Lake St. Martin</t>
+  </si>
+  <si>
+    <t>https://fnp-ppn.aadnc-aandc.gc.ca/fnp/Main/Search/FNPopulation.aspx?BAND_NUMBER=275&amp;lang=eng</t>
+  </si>
+  <si>
+    <t>Keeseekoowenin</t>
+  </si>
+  <si>
+    <t>https://fnp-ppn.aadnc-aandc.gc.ca/fnp/Main/Search/FNPopulation.aspx?BAND_NUMBER=286&amp;lang=eng</t>
   </si>
 </sst>
 </file>
@@ -429,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD62B1D0-367A-8B41-A5A1-C0871A73A6D6}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,12 +635,60 @@
         <v>https://fnp-ppn.aadnc-aandc.gc.ca/fnp/Main/Search/FNPopulation.aspx?BAND_NUMBER=295&amp;lang=eng</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>275</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>286</v>
+      </c>
+      <c r="C12">
+        <v>140</v>
+      </c>
+      <c r="D12">
+        <v>385</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="bfb77542-f000-416e-9391-d4f3ed66f756" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b313e45-d48c-4d36-b475-2ce2b8c74c54">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0E76F91975C3B469A9C9E5B90195820" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d044a0b9c54eefe6672bdcd1de2a28d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b313e45-d48c-4d36-b475-2ce2b8c74c54" xmlns:ns3="bfb77542-f000-416e-9391-d4f3ed66f756" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d9534cf13e5bbdf06d33948ab5fbaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="2b313e45-d48c-4d36-b475-2ce2b8c74c54"/>
@@ -871,34 +931,46 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{209BF923-FAAC-4167-925A-7A80DCDAE788}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="bfb77542-f000-416e-9391-d4f3ed66f756" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2b313e45-d48c-4d36-b475-2ce2b8c74c54">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EBC699E-C0C9-441B-ADE5-F21F0251997D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="bfb77542-f000-416e-9391-d4f3ed66f756"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2b313e45-d48c-4d36-b475-2ce2b8c74c54"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB8EDFA4-66DA-40C2-8599-D29D4F3A4EA4}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{209BF923-FAAC-4167-925A-7A80DCDAE788}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6EBC699E-C0C9-441B-ADE5-F21F0251997D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB8EDFA4-66DA-40C2-8599-D29D4F3A4EA4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b313e45-d48c-4d36-b475-2ce2b8c74c54"/>
+    <ds:schemaRef ds:uri="bfb77542-f000-416e-9391-d4f3ed66f756"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>